<commit_message>
Added final calls Added Installer
</commit_message>
<xml_diff>
--- a/Documents/Neato.command.mapping.xlsx
+++ b/Documents/Neato.command.mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\delphi projects\NeatoToolio\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A71F4F1-552A-4247-8FF9-080D113F8838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FA895E-5456-411D-BEF1-92657D2CA065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{315D293B-4658-4632-BA6F-48C002BD5910}"/>
   </bookViews>
@@ -786,7 +786,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +817,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -885,7 +885,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>67</v>
       </c>
@@ -987,7 +987,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>88</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>90</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>92</v>
       </c>
@@ -1581,10 +1581,10 @@
         <v>62</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>62</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -1756,11 +1756,17 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E54" xr:uid="{718676AD-44F4-4C49-9DCC-F6CA68B5FC76}">
-    <filterColumn colId="4">
+    <filterColumn colId="1">
       <filters>
-        <filter val="n"/>
-        <filter val="s"/>
-        <filter val="y"/>
+        <filter val="Executes different test modes. Once set, press Start button to engage. (Test modes are mutually exclusive.)"/>
+        <filter val="Set the operation mode of the robot. (TestMode Only)"/>
+        <filter val="Sets California Energy Commission 10-CFR-430 Battery Charging System Test mode."/>
+        <filter val="Sets LDS rotation on or off. Can only be run in TestMode."/>
+        <filter val="Sets TestMode on or off. Some commands can only be run in TestMode."/>
+        <filter val="Sets the IEC Cleaning Test parameters"/>
+        <filter val="Sets the LCD to the specified display. (TestMode Only)"/>
+        <filter val="Sets the specified LED to on,off,blink, or dim. (TestMode Only)"/>
+        <filter val="Sets the specified motor to run in a direction at a requested speed. (TestMode Only)"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>